<commit_message>
generar nombre de archivo a partir de la clues de imss bienestar + periodo
</commit_message>
<xml_diff>
--- a/public/template.xlsx
+++ b/public/template.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\solicitudes-app\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A253AB88-AB9A-41CB-BA22-F7748DEFAA6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBEC3AA0-BDD3-44F5-8C03-68F4D1B4FEF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-45" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="articulos" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">articulos!$B$12:$F$12</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">articulos!$B$1:$F$12</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">articulos!$B$13:$F$13</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">articulos!$B$1:$F$13</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t xml:space="preserve">SOLICITUD DE INSUMOS </t>
   </si>
@@ -63,9 +63,6 @@
     <t xml:space="preserve">UNIDAD DE MEDIDA </t>
   </si>
   <si>
-    <t>RESPONSABLE DE RECURSOS MATERIALES</t>
-  </si>
-  <si>
     <t>SURTIDO CON</t>
   </si>
   <si>
@@ -79,13 +76,25 @@
   </si>
   <si>
     <t>{{E5}}</t>
+  </si>
+  <si>
+    <t>RESPONSABLE DE CAPTURA</t>
+  </si>
+  <si>
+    <t>{{E8}}</t>
+  </si>
+  <si>
+    <t>TIPO DE PEDIDO</t>
+  </si>
+  <si>
+    <t>{{E9}}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -107,12 +116,6 @@
     </font>
     <font>
       <sz val="8"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -432,21 +435,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="7" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="6" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
@@ -455,7 +458,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -464,7 +467,97 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="7" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="7" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="7" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="7" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="7" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="7" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -476,101 +569,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="8" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="8" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="8" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="8" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="8" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="8" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -790,11 +796,11 @@
   <sheetPr codeName="Sheet1">
     <tabColor rgb="FF4F6128"/>
   </sheetPr>
-  <dimension ref="B1:O12"/>
+  <dimension ref="B1:O13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="12" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B13" sqref="B13"/>
+      <pane ySplit="13" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E9" sqref="E9:F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -808,15 +814,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="C1" s="18"/>
-      <c r="D1" s="23" t="s">
+      <c r="B1" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="14"/>
+      <c r="D1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="24"/>
-      <c r="F1" s="25"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="21"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
@@ -824,11 +830,11 @@
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="19"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="28"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="24"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
@@ -836,11 +842,11 @@
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="19"/>
-      <c r="C3" s="20"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="31"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="27"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
@@ -848,69 +854,69 @@
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="2:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="19"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="32" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" s="33"/>
-      <c r="F4" s="34"/>
+      <c r="B4" s="15"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="29"/>
+      <c r="F4" s="30"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="3"/>
-      <c r="L4" s="13"/>
-      <c r="M4" s="13"/>
-      <c r="N4" s="13"/>
+      <c r="L4" s="43"/>
+      <c r="M4" s="43"/>
+      <c r="N4" s="43"/>
       <c r="O4" s="4"/>
     </row>
     <row r="5" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="19"/>
-      <c r="C5" s="20"/>
+      <c r="B5" s="15"/>
+      <c r="C5" s="16"/>
       <c r="D5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="35" t="s">
-        <v>13</v>
-      </c>
-      <c r="F5" s="36"/>
+      <c r="E5" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="32"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
       <c r="K5" s="3"/>
       <c r="L5" s="5"/>
-      <c r="M5" s="14"/>
-      <c r="N5" s="14"/>
+      <c r="M5" s="44"/>
+      <c r="N5" s="44"/>
       <c r="O5" s="4"/>
     </row>
     <row r="6" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="19"/>
-      <c r="C6" s="20"/>
+      <c r="B6" s="15"/>
+      <c r="C6" s="16"/>
       <c r="D6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="37"/>
-      <c r="F6" s="38"/>
+        <v>8</v>
+      </c>
+      <c r="E6" s="33"/>
+      <c r="F6" s="34"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
       <c r="K6" s="3"/>
       <c r="L6" s="5"/>
-      <c r="M6" s="15"/>
-      <c r="N6" s="15"/>
+      <c r="M6" s="45"/>
+      <c r="N6" s="45"/>
       <c r="O6" s="4"/>
     </row>
     <row r="7" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="19"/>
-      <c r="C7" s="20"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="16"/>
       <c r="D7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="47"/>
-      <c r="F7" s="48"/>
+        <v>9</v>
+      </c>
+      <c r="E7" s="41"/>
+      <c r="F7" s="42"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
@@ -922,113 +928,136 @@
       <c r="O7" s="4"/>
     </row>
     <row r="8" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="19"/>
-      <c r="C8" s="20"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="16"/>
       <c r="D8" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" s="39"/>
-      <c r="F8" s="40"/>
+        <v>15</v>
+      </c>
+      <c r="E8" s="41" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" s="47"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
       <c r="K8" s="3"/>
       <c r="L8" s="5"/>
-      <c r="M8" s="15"/>
-      <c r="N8" s="15"/>
+      <c r="M8" s="6"/>
+      <c r="N8" s="6"/>
       <c r="O8" s="4"/>
     </row>
-    <row r="9" spans="2:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="19"/>
-      <c r="C9" s="20"/>
-      <c r="D9" s="41" t="s">
-        <v>2</v>
-      </c>
-      <c r="E9" s="42"/>
-      <c r="F9" s="43"/>
+    <row r="9" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="15"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="48" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" s="49"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
       <c r="K9" s="3"/>
-      <c r="L9" s="7"/>
-      <c r="M9" s="16"/>
-      <c r="N9" s="16"/>
+      <c r="L9" s="5"/>
+      <c r="M9" s="45"/>
+      <c r="N9" s="45"/>
       <c r="O9" s="4"/>
     </row>
     <row r="10" spans="2:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="19"/>
-      <c r="C10" s="20"/>
-      <c r="D10" s="41"/>
-      <c r="E10" s="42"/>
-      <c r="F10" s="43"/>
+      <c r="B10" s="15"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="35" t="s">
+        <v>2</v>
+      </c>
+      <c r="E10" s="36"/>
+      <c r="F10" s="37"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
       <c r="K10" s="3"/>
       <c r="L10" s="7"/>
-      <c r="M10" s="8"/>
-      <c r="N10" s="8"/>
+      <c r="M10" s="46"/>
+      <c r="N10" s="46"/>
       <c r="O10" s="4"/>
     </row>
-    <row r="11" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B11" s="21"/>
-      <c r="C11" s="22"/>
-      <c r="D11" s="44"/>
-      <c r="E11" s="45"/>
-      <c r="F11" s="46"/>
+    <row r="11" spans="2:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="15"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="35"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="37"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
       <c r="K11" s="3"/>
-      <c r="L11" s="4"/>
-      <c r="M11" s="4"/>
-      <c r="N11" s="4"/>
+      <c r="L11" s="7"/>
+      <c r="M11" s="8"/>
+      <c r="N11" s="8"/>
       <c r="O11" s="4"/>
     </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B12" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="D12" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="E12" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="F12" s="11" t="s">
-        <v>6</v>
-      </c>
+    <row r="12" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B12" s="17"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="38"/>
+      <c r="E12" s="39"/>
+      <c r="F12" s="40"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
-      <c r="K12" s="1"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="4"/>
+      <c r="M12" s="4"/>
+      <c r="N12" s="4"/>
+      <c r="O12" s="4"/>
+    </row>
+    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B13" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="B12:F12" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
-  <mergeCells count="15">
-    <mergeCell ref="B1:C11"/>
+  <autoFilter ref="B13:F13" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <mergeCells count="16">
+    <mergeCell ref="L4:N4"/>
+    <mergeCell ref="M5:N5"/>
+    <mergeCell ref="M6:N6"/>
+    <mergeCell ref="M9:N9"/>
+    <mergeCell ref="M10:N10"/>
+    <mergeCell ref="B1:C12"/>
     <mergeCell ref="D1:F3"/>
     <mergeCell ref="D4:F4"/>
     <mergeCell ref="E5:F5"/>
     <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="D12:F12"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="D11:F11"/>
     <mergeCell ref="E8:F8"/>
-    <mergeCell ref="D9:F9"/>
-    <mergeCell ref="D11:F11"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="D10:F10"/>
-    <mergeCell ref="L4:N4"/>
-    <mergeCell ref="M5:N5"/>
-    <mergeCell ref="M6:N6"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="M9:N9"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967294" verticalDpi="4294967294" r:id="rId1"/>

</xml_diff>

<commit_message>
fixes de template al exportar
</commit_message>
<xml_diff>
--- a/public/template.xlsx
+++ b/public/template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\solicitudes-app\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3FAED3B-0DC5-45E5-A85D-FDF3208129B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45377106-6686-4044-A3F0-ACBC0896FB72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-45" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -498,8 +498,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -582,34 +591,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -903,7 +903,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="13" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E22" sqref="E22"/>
+      <selection pane="bottomLeft" activeCell="B1" sqref="B1:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -917,15 +917,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="50" t="e" vm="1">
+      <c r="B1" s="49" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
-      <c r="C1" s="49"/>
-      <c r="D1" s="14" t="s">
+      <c r="C1" s="50"/>
+      <c r="D1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="15"/>
-      <c r="F1" s="16"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="19"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
@@ -933,11 +933,11 @@
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="2:15" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="50"/>
-      <c r="C2" s="49"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="19"/>
+      <c r="B2" s="49"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="22"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
@@ -945,11 +945,11 @@
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="2:15" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="50"/>
-      <c r="C3" s="49"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="22"/>
+      <c r="B3" s="49"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="25"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
@@ -957,23 +957,23 @@
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="2:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="44" t="s">
         <v>16</v>
       </c>
       <c r="C4" s="45"/>
-      <c r="D4" s="23" t="s">
+      <c r="D4" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="24"/>
-      <c r="F4" s="25"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="28"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="3"/>
-      <c r="L4" s="41"/>
-      <c r="M4" s="41"/>
-      <c r="N4" s="41"/>
+      <c r="L4" s="13"/>
+      <c r="M4" s="13"/>
+      <c r="N4" s="13"/>
       <c r="O4" s="4"/>
     </row>
     <row r="5" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -982,18 +982,18 @@
       <c r="D5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="26" t="s">
+      <c r="E5" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="27"/>
+      <c r="F5" s="30"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
       <c r="K5" s="3"/>
       <c r="L5" s="5"/>
-      <c r="M5" s="42"/>
-      <c r="N5" s="42"/>
+      <c r="M5" s="14"/>
+      <c r="N5" s="14"/>
       <c r="O5" s="4"/>
     </row>
     <row r="6" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1002,16 +1002,16 @@
       <c r="D6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="28"/>
-      <c r="F6" s="29"/>
+      <c r="E6" s="31"/>
+      <c r="F6" s="32"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
       <c r="K6" s="3"/>
       <c r="L6" s="5"/>
-      <c r="M6" s="43"/>
-      <c r="N6" s="43"/>
+      <c r="M6" s="15"/>
+      <c r="N6" s="15"/>
       <c r="O6" s="4"/>
     </row>
     <row r="7" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1020,8 +1020,8 @@
       <c r="D7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="38"/>
-      <c r="F7" s="39"/>
+      <c r="E7" s="41"/>
+      <c r="F7" s="42"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
@@ -1038,10 +1038,10 @@
       <c r="D8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E8" s="38" t="s">
+      <c r="E8" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="F8" s="40"/>
+      <c r="F8" s="43"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
@@ -1058,44 +1058,44 @@
       <c r="D9" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="30" t="s">
+      <c r="E9" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="F9" s="31"/>
+      <c r="F9" s="34"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
       <c r="K9" s="3"/>
       <c r="L9" s="5"/>
-      <c r="M9" s="43"/>
-      <c r="N9" s="43"/>
+      <c r="M9" s="15"/>
+      <c r="N9" s="15"/>
       <c r="O9" s="4"/>
     </row>
     <row r="10" spans="2:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="46"/>
       <c r="C10" s="45"/>
-      <c r="D10" s="32" t="s">
+      <c r="D10" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="E10" s="33"/>
-      <c r="F10" s="34"/>
+      <c r="E10" s="36"/>
+      <c r="F10" s="37"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
       <c r="K10" s="3"/>
       <c r="L10" s="7"/>
-      <c r="M10" s="44"/>
-      <c r="N10" s="44"/>
+      <c r="M10" s="16"/>
+      <c r="N10" s="16"/>
       <c r="O10" s="4"/>
     </row>
     <row r="11" spans="2:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="46"/>
       <c r="C11" s="45"/>
-      <c r="D11" s="32"/>
-      <c r="E11" s="33"/>
-      <c r="F11" s="34"/>
+      <c r="D11" s="35"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="37"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
@@ -1109,9 +1109,9 @@
     <row r="12" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B12" s="47"/>
       <c r="C12" s="48"/>
-      <c r="D12" s="35"/>
-      <c r="E12" s="36"/>
-      <c r="F12" s="37"/>
+      <c r="D12" s="38"/>
+      <c r="E12" s="39"/>
+      <c r="F12" s="40"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
@@ -1147,23 +1147,23 @@
   </sheetData>
   <autoFilter ref="B13:F13" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <mergeCells count="17">
+    <mergeCell ref="B4:C12"/>
+    <mergeCell ref="B1:C3"/>
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="D12:F12"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="D11:F11"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="D1:F3"/>
+    <mergeCell ref="D4:F4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E9:F9"/>
     <mergeCell ref="L4:N4"/>
     <mergeCell ref="M5:N5"/>
     <mergeCell ref="M6:N6"/>
     <mergeCell ref="M9:N9"/>
     <mergeCell ref="M10:N10"/>
-    <mergeCell ref="D1:F3"/>
-    <mergeCell ref="D4:F4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="D10:F10"/>
-    <mergeCell ref="D12:F12"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="D11:F11"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="B4:C12"/>
-    <mergeCell ref="B1:C3"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967294" verticalDpi="4294967294" r:id="rId1"/>

</xml_diff>

<commit_message>
Mejoras listas para testear
</commit_message>
<xml_diff>
--- a/public/template.xlsx
+++ b/public/template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\solicitudes-app\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCF90E38-4F9D-4290-8E7E-DA6F379542C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{511B224F-ED31-4259-B744-A9CACD8B562C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t xml:space="preserve">SOLICITUD DE INSUMOS </t>
   </si>
@@ -110,13 +110,25 @@
   </si>
   <si>
     <t>{{F5}}</t>
+  </si>
+  <si>
+    <t>Existencias</t>
+  </si>
+  <si>
+    <t>AZM</t>
+  </si>
+  <si>
+    <t>AZT</t>
+  </si>
+  <si>
+    <t>AZE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -185,8 +197,15 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -205,8 +224,14 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDDD9C3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="23">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -447,6 +472,21 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -456,7 +496,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -485,12 +525,54 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -571,39 +653,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -613,6 +662,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFDDD9C3"/>
       <color rgb="FF006341"/>
     </mruColors>
   </colors>
@@ -897,31 +947,31 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="11" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
+      <selection pane="bottomLeft" activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.42578125" customWidth="1"/>
-    <col min="2" max="2" width="3.85546875" style="11" customWidth="1"/>
-    <col min="3" max="3" width="14.140625" style="11" customWidth="1"/>
-    <col min="4" max="4" width="16.85546875" customWidth="1"/>
+    <col min="2" max="2" width="4.28515625" style="11" customWidth="1"/>
+    <col min="3" max="3" width="8.42578125" style="11" customWidth="1"/>
+    <col min="4" max="4" width="18" customWidth="1"/>
     <col min="5" max="5" width="37.85546875" customWidth="1"/>
     <col min="6" max="6" width="14.7109375" customWidth="1"/>
     <col min="7" max="7" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="12" t="e" vm="1">
+      <c r="B1" s="27" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
-      <c r="C1" s="13"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="25" t="s">
+      <c r="C1" s="16"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="26"/>
-      <c r="G1" s="27"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="41"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
@@ -929,12 +979,12 @@
       <c r="L1" s="1"/>
     </row>
     <row r="2" spans="2:16" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="12"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="30"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="44"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
@@ -942,12 +992,12 @@
       <c r="L2" s="1"/>
     </row>
     <row r="3" spans="2:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="12"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="31"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="33"/>
+      <c r="B3" s="27"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="45"/>
+      <c r="F3" s="46"/>
+      <c r="G3" s="47"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
@@ -955,56 +1005,56 @@
       <c r="L3" s="1"/>
     </row>
     <row r="4" spans="2:16" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="44" t="s">
+      <c r="B4" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="45"/>
-      <c r="D4" s="46"/>
-      <c r="E4" s="34" t="s">
+      <c r="C4" s="18"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="35"/>
-      <c r="G4" s="36"/>
+      <c r="F4" s="49"/>
+      <c r="G4" s="50"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
       <c r="L4" s="3"/>
-      <c r="M4" s="41"/>
-      <c r="N4" s="41"/>
-      <c r="O4" s="41"/>
+      <c r="M4" s="13"/>
+      <c r="N4" s="13"/>
+      <c r="O4" s="13"/>
       <c r="P4" s="4"/>
     </row>
     <row r="5" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="47"/>
-      <c r="C5" s="48"/>
-      <c r="D5" s="46"/>
+      <c r="B5" s="20"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="19"/>
       <c r="E5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="F5" s="37" t="s">
+      <c r="F5" s="51" t="s">
         <v>16</v>
       </c>
-      <c r="G5" s="38"/>
+      <c r="G5" s="52"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
       <c r="L5" s="3"/>
       <c r="M5" s="5"/>
-      <c r="N5" s="42"/>
-      <c r="O5" s="42"/>
+      <c r="N5" s="14"/>
+      <c r="O5" s="14"/>
       <c r="P5" s="4"/>
     </row>
     <row r="6" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="47"/>
-      <c r="C6" s="48"/>
-      <c r="D6" s="46"/>
+      <c r="B6" s="20"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="19"/>
       <c r="E6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="21"/>
-      <c r="G6" s="22"/>
+      <c r="F6" s="35"/>
+      <c r="G6" s="36"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
@@ -1016,16 +1066,16 @@
       <c r="P6" s="4"/>
     </row>
     <row r="7" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="47"/>
-      <c r="C7" s="48"/>
-      <c r="D7" s="46"/>
+      <c r="B7" s="20"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="19"/>
       <c r="E7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="23" t="s">
+      <c r="F7" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="G7" s="24"/>
+      <c r="G7" s="38"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
@@ -1037,55 +1087,57 @@
       <c r="P7" s="4"/>
     </row>
     <row r="8" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="47"/>
-      <c r="C8" s="48"/>
-      <c r="D8" s="46"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="19"/>
       <c r="E8" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F8" s="39" t="s">
+      <c r="F8" s="53" t="s">
         <v>15</v>
       </c>
-      <c r="G8" s="40"/>
+      <c r="G8" s="54"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
       <c r="L8" s="3"/>
       <c r="M8" s="5"/>
-      <c r="N8" s="43"/>
-      <c r="O8" s="43"/>
+      <c r="N8" s="15"/>
+      <c r="O8" s="15"/>
       <c r="P8" s="4"/>
     </row>
     <row r="9" spans="2:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="47"/>
-      <c r="C9" s="48"/>
-      <c r="D9" s="46"/>
-      <c r="E9" s="15" t="s">
+      <c r="B9" s="20"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="F9" s="16"/>
-      <c r="G9" s="17"/>
+      <c r="F9" s="30"/>
+      <c r="G9" s="31"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
       <c r="L9" s="3"/>
       <c r="M9" s="7"/>
-      <c r="N9" s="13"/>
-      <c r="O9" s="13"/>
+      <c r="N9" s="16"/>
+      <c r="O9" s="16"/>
       <c r="P9" s="4"/>
     </row>
     <row r="10" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B10" s="49"/>
-      <c r="C10" s="50"/>
-      <c r="D10" s="51"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="19"/>
-      <c r="G10" s="20"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
+      <c r="B10" s="22"/>
+      <c r="C10" s="23"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="32"/>
+      <c r="F10" s="33"/>
+      <c r="G10" s="34"/>
+      <c r="H10" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="I10" s="26"/>
+      <c r="J10" s="26"/>
       <c r="K10" s="1"/>
       <c r="L10" s="3"/>
       <c r="M10" s="4"/>
@@ -1112,20 +1164,21 @@
       <c r="G11" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
+      <c r="H11" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="I11" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="J11" s="12" t="s">
+        <v>20</v>
+      </c>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
     </row>
   </sheetData>
   <autoFilter ref="B11:G11" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
-  <mergeCells count="14">
-    <mergeCell ref="M4:O4"/>
-    <mergeCell ref="N5:O5"/>
-    <mergeCell ref="N8:O8"/>
-    <mergeCell ref="N9:O9"/>
-    <mergeCell ref="B4:D10"/>
+  <mergeCells count="15">
     <mergeCell ref="B1:D3"/>
     <mergeCell ref="E9:G9"/>
     <mergeCell ref="E10:G10"/>
@@ -1135,6 +1188,12 @@
     <mergeCell ref="E4:G4"/>
     <mergeCell ref="F5:G5"/>
     <mergeCell ref="F8:G8"/>
+    <mergeCell ref="M4:O4"/>
+    <mergeCell ref="N5:O5"/>
+    <mergeCell ref="N8:O8"/>
+    <mergeCell ref="N9:O9"/>
+    <mergeCell ref="B4:D10"/>
+    <mergeCell ref="H10:J10"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup fitToHeight="0" orientation="portrait" horizontalDpi="4294967294" verticalDpi="4294967294" r:id="rId1"/>

</xml_diff>